<commit_message>
common logging correlation 5 and 6
</commit_message>
<xml_diff>
--- a/correlation/correlation 5 and 6 - commons-logging .xlsx
+++ b/correlation/correlation 5 and 6 - commons-logging .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sl.No</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Metrics 6</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
-    <t>1.0.3</t>
   </si>
   <si>
     <t>1.0.4</t>
@@ -56,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -78,6 +72,7 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -123,10 +118,13 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -376,11 +374,11 @@
         <v>7</v>
       </c>
       <c r="C5" s="4">
-        <v>308.0</v>
+        <v>993.0</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D12" si="1">78+(0.01*C5)</f>
-        <v>81.08</v>
+        <f t="shared" ref="D5:D10" si="1">78+(0.01*C5)</f>
+        <v>87.93</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -390,15 +388,15 @@
       <c r="A6" s="3">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
+      <c r="B6" s="5">
+        <v>1.1</v>
       </c>
       <c r="C6" s="4">
-        <v>1132.0</v>
+        <v>4157.0</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>89.32</v>
+        <v>119.57</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -409,14 +407,14 @@
         <v>3.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>993.0</v>
+        <v>568.0</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>87.93</v>
+        <v>83.68</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -426,15 +424,15 @@
       <c r="A8" s="3">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
-        <v>1.1</v>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="4">
-        <v>4157.0</v>
+        <v>5806.0</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>119.57</v>
+        <v>136.06</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -448,11 +446,11 @@
         <v>10</v>
       </c>
       <c r="C9" s="4">
-        <v>568.0</v>
+        <v>0.0</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>83.68</v>
+        <v>78</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -462,79 +460,61 @@
       <c r="A10" s="3">
         <v>6.0</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
+      <c r="B10" s="4">
+        <v>1.2</v>
       </c>
       <c r="C10" s="4">
-        <v>5806.0</v>
+        <v>83.0</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="1"/>
-        <v>136.06</v>
+        <v>78.83</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="C12" s="4">
-        <v>83.0</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
-        <v>78.83</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>

</xml_diff>